<commit_message>
Agrega advertencia visual para ligas con menos de 5 fechas
</commit_message>
<xml_diff>
--- a/Ligas/Liga_peruana_2025.xlsx
+++ b/Ligas/Liga_peruana_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3900D41-91F6-48C3-927F-F71D913CE48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CADFB17-7178-4BF7-A503-3919FC7BFCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -761,6 +761,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>